<commit_message>
Apply two more fixes
</commit_message>
<xml_diff>
--- a/data/problematic_sites_1_0_0.xlsx
+++ b/data/problematic_sites_1_0_0.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="275">
   <si>
     <t xml:space="preserve">TSid</t>
   </si>
@@ -818,6 +818,33 @@
   </si>
   <si>
     <t xml:space="preserve">Use top sample for anomaly? Hol average is -31C, top sample is -30.5C and 43BP. See the other GISP2 record Alley.GISP2.2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2L_MD97_2120_d18o_bulloides_SST_from_d18o_bulloides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MD97_2120.Pahnke.2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a one of those unreviewed 18O records. It has large 2-3C offset with Alkenone and Mg/Ca records from same core, which I would trust more as they have been carefully reviewed by the original authors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ReEnzeIOExA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LakePupuke.Pollen.NewZealand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> I just checked and Darrell appears to have chosen the PLS (~13.5C Holocene average) reconstruction to include in climate12k instead of the MAAT (~14.5C Holocene average), which is favoured by the authors. Maybe he was confusing the the PLS pollen reconstruction with the WAPLS chironomid reconstruction in the same paper. Anyway, the authors definitely favour the MAAT pollen reconstruction so we should use that one.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPZj5YKrFr0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include and use authors modern temperature of 15C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">see ReEnzeIOExA.  For information, the paper gives the modern value at the site as 15C, which we could use instead of worldclim</t>
   </si>
 </sst>
 </file>
@@ -833,7 +860,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -919,22 +945,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A71" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B98" activeCellId="0" sqref="B98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A81" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D108" activeCellId="0" sqref="D108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="15.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="75.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="75.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="6" style="0" width="10.61"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2722,7 +2749,57 @@
         <v>265</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>